<commit_message>
Beispiele, Modell und Code im docs Ordner
</commit_message>
<xml_diff>
--- a/order/MBSE Demonstrator Materialliste.xlsx
+++ b/order/MBSE Demonstrator Materialliste.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mimeiners/Documents/courses/prj/sose23/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mimeiners/Documents/courses/prj/sose23/gimbal/order/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF0A4A9-D614-5943-8F5F-71D376569B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D877E4-56AA-804E-851B-61EF714DF021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3140" yWindow="600" windowWidth="36840" windowHeight="23340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,7 +136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,16 +152,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -169,12 +182,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -184,8 +213,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Berechnung" xfId="2" builtinId="22"/>
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -468,7 +499,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -544,7 +575,7 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="5">
         <f>F4*G4</f>
         <v>2.99</v>
       </c>
@@ -586,7 +617,7 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <f>F6*G6</f>
         <v>4.1500000000000004</v>
       </c>
@@ -607,7 +638,7 @@
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="5">
         <f t="shared" ref="H7:H10" si="0">F7*G7</f>
         <v>0.99</v>
       </c>
@@ -628,7 +659,7 @@
       <c r="G8">
         <v>4</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="5">
         <f t="shared" si="0"/>
         <v>19.600000000000001</v>
       </c>
@@ -717,7 +748,7 @@
         <v>10.85</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -733,7 +764,7 @@
       <c r="G13">
         <v>1</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="5">
         <f>F13*G13</f>
         <v>20.99</v>
       </c>

</xml_diff>